<commit_message>
✅ Update automático XLSX
</commit_message>
<xml_diff>
--- a/stock_critico_master.xlsx
+++ b/stock_critico_master.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://galileacl-my.sharepoint.com/personal/benjamin_espinoza_galilea_cl/Documents/Escritorio/nueva actualziacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_7BB9675F5C7D880E62355476585DCE3A87439997" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A39B69E-73AA-40A4-BB32-D4F96F502DBD}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_7BB9675F5C7D880E62355476585DCE3A87439997" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28CA144E-36E7-43D0-B0B8-CD2A9967058B}"/>
   <bookViews>
     <workbookView xWindow="-3915" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Stock QR" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$443</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Stock QR'!$A$1:$K$443</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>